<commit_message>
upload fix img not update
</commit_message>
<xml_diff>
--- a/src/main/webapp/document/houses.xlsx
+++ b/src/main/webapp/document/houses.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="61">
   <si>
     <t>STT</t>
   </si>
@@ -102,37 +102,40 @@
     <t>14/2 Gio An - P.5 - TP.Đà Lạt</t>
   </si>
   <si>
+    <t>VILLA TẦM TRUNG</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&amp;nbsp;&lt;span style="background-color:rgb(255,255,255);color:rgb(13,13,13);font-family:Söhne, ui-sans-serif, system-ui, -apple-system, &amp;quot;Segoe UI&amp;quot;, Roboto, Ubuntu, Cantarell, &amp;quot;Noto Sans&amp;quot;, sans-serif, &amp;quot;Helvetica Neue&amp;quot;, Arial, &amp;quot;Apple Color Emoji&amp;quot;, &amp;quot;Segoe UI Emoji&amp;quot;, &amp;quot;Segoe UI Symbol&amp;quot;, &amp;quot;Noto Color Emoji&amp;quot;;font-size:16px;"&gt;&lt;span style="-webkit-text-stroke-width:0px;display:inline !important;float:none;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:normal;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;Dạo này, mọi người đang cảm thấy mệt mỏi với nhịp sống hối hả và tiêu cực? Đừng lo lắng nữa! Hãy để Homestay Đà Lạt HS3 là điểm dừng chân lý tưởng của bạn để tìm lại sự bình yên và hạnh phúc!&amp;nbsp;&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;&lt;p style="--tw-backdrop-blur:;--tw-backdrop-brightness:;--tw-backdrop-contrast:;--tw-backdrop-grayscale:;--tw-backdrop-hue-rotate:;--tw-backdrop-invert:;--tw-backdrop-opacity:;--tw-backdrop-saturate:;--tw-backdrop-sepia:;--tw-blur:;--tw-border-spacing-x:0;--tw-border-spacing-y:0;--tw-brightness:;--tw-contrast:;--tw-drop-shadow:;--tw-gradient-from-position:;--tw-gradient-to-position:;--tw-gradient-via-position:;--tw-grayscale:;--tw-hue-rotate:;--tw-invert:;--tw-numeric-figure:;--tw-numeric-fraction:;--tw-numeric-spacing:;--tw-ordinal:;--tw-pan-x:;--tw-pan-y:;--tw-pinch-zoom:;--tw-ring-color:rgba(69,89,164,.5);--tw-ring-inset:;--tw-ring-offset-color:#fff;--tw-ring-offset-shadow:0 0 transparent;--tw-ring-offset-width:0px;--tw-ring-shadow:0 0 transparent;--tw-rotate:0;--tw-saturate:;--tw-scale-x:1;--tw-scale-y:1;--tw-scroll-snap-strictness:proximity;--tw-sepia:;--tw-shadow-colored:0 0 transparent;--tw-shadow:0 0 transparent;--tw-skew-x:0;--tw-skew-y:0;--tw-slashed-zero:;--tw-translate-x:0;--tw-translate-y:0;-webkit-text-stroke-width:0px;background-color:rgb(255, 255, 255);border:0px solid rgb(227, 227, 227);box-sizing:border-box;color:rgb(13, 13, 13);font-family:Söhne, ui-sans-serif, system-ui, -apple-system, &amp;quot;Segoe UI&amp;quot;, Roboto, Ubuntu, Cantarell, &amp;quot;Noto Sans&amp;quot;, sans-serif, &amp;quot;Helvetica Neue&amp;quot;, Arial, &amp;quot;Apple Color Emoji&amp;quot;, &amp;quot;Segoe UI Emoji&amp;quot;, &amp;quot;Segoe UI Symbol&amp;quot;, &amp;quot;Noto Color Emoji&amp;quot;;font-size:16px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:normal;margin:1.25em 0px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;📌 Cơ cấu: 3 phòng ngủ - 3 toilet, thiết kế sang trọng và ấm cúng.&amp;nbsp;&lt;/p&gt;&lt;p style="--tw-backdrop-blur:;--tw-backdrop-brightness:;--tw-backdrop-contrast:;--tw-backdrop-grayscale:;--tw-backdrop-hue-rotate:;--tw-backdrop-invert:;--tw-backdrop-opacity:;--tw-backdrop-saturate:;--tw-backdrop-sepia:;--tw-blur:;--tw-border-spacing-x:0;--tw-border-spacing-y:0;--tw-brightness:;--tw-contrast:;--tw-drop-shadow:;--tw-gradient-from-position:;--tw-gradient-to-position:;--tw-gradient-via-position:;--tw-grayscale:;--tw-hue-rotate:;--tw-invert:;--tw-numeric-figure:;--tw-numeric-fraction:;--tw-numeric-spacing:;--tw-ordinal:;--tw-pan-x:;--tw-pan-y:;--tw-pinch-zoom:;--tw-ring-color:rgba(69,89,164,.5);--tw-ring-inset:;--tw-ring-offset-color:#fff;--tw-ring-offset-shadow:0 0 transparent;--tw-ring-offset-width:0px;--tw-ring-shadow:0 0 transparent;--tw-rotate:0;--tw-saturate:;--tw-scale-x:1;--tw-scale-y:1;--tw-scroll-snap-strictness:proximity;--tw-sepia:;--tw-shadow-colored:0 0 transparent;--tw-shadow:0 0 transparent;--tw-skew-x:0;--tw-skew-y:0;--tw-slashed-zero:;--tw-translate-x:0;--tw-translate-y:0;-webkit-text-stroke-width:0px;background-color:rgb(255, 255, 255);border:0px solid rgb(227, 227, 227);box-sizing:border-box;color:rgb(13, 13, 13);font-family:Söhne, ui-sans-serif, system-ui, -apple-system, &amp;quot;Segoe UI&amp;quot;, Roboto, Ubuntu, Cantarell, &amp;quot;Noto Sans&amp;quot;, sans-serif, &amp;quot;Helvetica Neue&amp;quot;, Arial, &amp;quot;Apple Color Emoji&amp;quot;, &amp;quot;Segoe UI Emoji&amp;quot;, &amp;quot;Segoe UI Symbol&amp;quot;, &amp;quot;Noto Color Emoji&amp;quot;;font-size:16px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:normal;margin:1.25em 0px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;👩‍🍳 Bếp Ngọt Ngào: Không gian bếp ấm áp với những dụng cụ nấu nướng đầy đủ, cho bạn tự do sáng tạo và thưởng thức những món ngon.&lt;/p&gt;&lt;p style="--tw-backdrop-blur:;--tw-backdrop-brightness:;--tw-backdrop-contrast:;--tw-backdrop-grayscale:;--tw-backdrop-hue-rotate:;--tw-backdrop-invert:;--tw-backdrop-opacity:;--tw-backdrop-saturate:;--tw-backdrop-sepia:;--tw-blur:;--tw-border-spacing-x:0;--tw-border-spacing-y:0;--tw-brightness:;--tw-contrast:;--tw-drop-shadow:;--tw-gradient-from-position:;--tw-gradient-to-position:;--tw-gradient-via-position:;--tw-grayscale:;--tw-hue-rotate:;--tw-invert:;--tw-numeric-figure:;--tw-numeric-fraction:;--tw-numeric-spacing:;--tw-ordinal:;--tw-pan-x:;--tw-pan-y:;--tw-pinch-zoom:;--tw-ring-color:rgba(69,89,164,.5);--tw-ring-inset:;--tw-ring-offset-color:#fff;--tw-ring-offset-shadow:0 0 transparent;--tw-ring-offset-width:0px;--tw-ring-shadow:0 0 transparent;--tw-rotate:0;--tw-saturate:;--tw-scale-x:1;--tw-scale-y:1;--tw-scroll-snap-strictness:proximity;--tw-sepia:;--tw-shadow-colored:0 0 transparent;--tw-shadow:0 0 transparent;--tw-skew-x:0;--tw-skew-y:0;--tw-slashed-zero:;--tw-translate-x:0;--tw-translate-y:0;-webkit-text-stroke-width:0px;background-color:rgb(255, 255, 255);border:0px solid rgb(227, 227, 227);box-sizing:border-box;color:rgb(13, 13, 13);font-family:Söhne, ui-sans-serif, system-ui, -apple-system, &amp;quot;Segoe UI&amp;quot;, Roboto, Ubuntu, Cantarell, &amp;quot;Noto Sans&amp;quot;, sans-serif, &amp;quot;Helvetica Neue&amp;quot;, Arial, &amp;quot;Apple Color Emoji&amp;quot;, &amp;quot;Segoe UI Emoji&amp;quot;, &amp;quot;Segoe UI Symbol&amp;quot;, &amp;quot;Noto Color Emoji&amp;quot;;font-size:16px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:normal;margin:1.25em 0px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;&amp;nbsp;🫶🏻 Sân BBQ : Sân BBQ thoáng đãng, là nơi lý tưởng cho các buổi tiệc nướng vui vẻ và đầy ấm áp.&amp;nbsp;&lt;/p&gt;&lt;p style="--tw-backdrop-blur:;--tw-backdrop-brightness:;--tw-backdrop-contrast:;--tw-backdrop-grayscale:;--tw-backdrop-hue-rotate:;--tw-backdrop-invert:;--tw-backdrop-opacity:;--tw-backdrop-saturate:;--tw-backdrop-sepia:;--tw-blur:;--tw-border-spacing-x:0;--tw-border-spacing-y:0;--tw-brightness:;--tw-contrast:;--tw-drop-shadow:;--tw-gradient-from-position:;--tw-gradient-to-position:;--tw-gradient-via-position:;--tw-grayscale:;--tw-hue-rotate:;--tw-invert:;--tw-numeric-figure:;--tw-numeric-fraction:;--tw-numeric-spacing:;--tw-ordinal:;--tw-pan-x:;--tw-pan-y:;--tw-pinch-zoom:;--tw-ring-color:rgba(69,89,164,.5);--tw-ring-inset:;--tw-ring-offset-color:#fff;--tw-ring-offset-shadow:0 0 transparent;--tw-ring-offset-width:0px;--tw-ring-shadow:0 0 transparent;--tw-rotate:0;--tw-saturate:;--tw-scale-x:1;--tw-scale-y:1;--tw-scroll-snap-strictness:proximity;--tw-sepia:;--tw-shadow-colored:0 0 transparent;--tw-shadow:0 0 transparent;--tw-skew-x:0;--tw-skew-y:0;--tw-slashed-zero:;--tw-translate-x:0;--tw-translate-y:0;-webkit-text-stroke-width:0px;background-color:rgb(255, 255, 255);border:0px solid rgb(227, 227, 227);box-sizing:border-box;color:rgb(13, 13, 13);font-family:Söhne, ui-sans-serif, system-ui, -apple-system, &amp;quot;Segoe UI&amp;quot;, Roboto, Ubuntu, Cantarell, &amp;quot;Noto Sans&amp;quot;, sans-serif, &amp;quot;Helvetica Neue&amp;quot;, Arial, &amp;quot;Apple Color Emoji&amp;quot;, &amp;quot;Segoe UI Emoji&amp;quot;, &amp;quot;Segoe UI Symbol&amp;quot;, &amp;quot;Noto Color Emoji&amp;quot;;font-size:16px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:normal;margin:1.25em 0px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;📌 Máy Nước Nóng: Sẵn có nước nóng 24/7, đảm bảo bạn luôn cảm thấy thoải mái và thư giãn.&amp;nbsp;&lt;/p&gt;&lt;p style="--tw-backdrop-blur:;--tw-backdrop-brightness:;--tw-backdrop-contrast:;--tw-backdrop-grayscale:;--tw-backdrop-hue-rotate:;--tw-backdrop-invert:;--tw-backdrop-opacity:;--tw-backdrop-saturate:;--tw-backdrop-sepia:;--tw-blur:;--tw-border-spacing-x:0;--tw-border-spacing-y:0;--tw-brightness:;--tw-contrast:;--tw-drop-shadow:;--tw-gradient-from-position:;--tw-gradient-to-position:;--tw-gradient-via-position:;--tw-grayscale:;--tw-hue-rotate:;--tw-invert:;--tw-numeric-figure:;--tw-numeric-fraction:;--tw-numeric-spacing:;--tw-ordinal:;--tw-pan-x:;--tw-pan-y:;--tw-pinch-zoom:;--tw-ring-color:rgba(69,89,164,.5);--tw-ring-inset:;--tw-ring-offset-color:#fff;--tw-ring-offset-shadow:0 0 transparent;--tw-ring-offset-width:0px;--tw-ring-shadow:0 0 transparent;--tw-rotate:0;--tw-saturate:;--tw-scale-x:1;--tw-scale-y:1;--tw-scroll-snap-strictness:proximity;--tw-sepia:;--tw-shadow-colored:0 0 transparent;--tw-shadow:0 0 transparent;--tw-skew-x:0;--tw-skew-y:0;--tw-slashed-zero:;--tw-translate-x:0;--tw-translate-y:0;-webkit-text-stroke-width:0px;background-color:rgb(255, 255, 255);border:0px solid rgb(227, 227, 227);box-sizing:border-box;color:rgb(13, 13, 13);font-family:Söhne, ui-sans-serif, system-ui, -apple-system, &amp;quot;Segoe UI&amp;quot;, Roboto, Ubuntu, Cantarell, &amp;quot;Noto Sans&amp;quot;, sans-serif, &amp;quot;Helvetica Neue&amp;quot;, Arial, &amp;quot;Apple Color Emoji&amp;quot;, &amp;quot;Segoe UI Emoji&amp;quot;, &amp;quot;Segoe UI Symbol&amp;quot;, &amp;quot;Noto Color Emoji&amp;quot;;font-size:16px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:normal;margin:1.25em 0px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;📌 Đèn Chiếu Sáng: Hãy thư giãn dưới ánh đèn màu vàng ấm áp, tạo không gian lý tưởng cho việc đọc sách và tận hưởng khoảnh khắc riêng tư.&amp;nbsp;&lt;/p&gt;&lt;p style="--tw-backdrop-blur:;--tw-backdrop-brightness:;--tw-backdrop-contrast:;--tw-backdrop-grayscale:;--tw-backdrop-hue-rotate:;--tw-backdrop-invert:;--tw-backdrop-opacity:;--tw-backdrop-saturate:;--tw-backdrop-sepia:;--tw-blur:;--tw-border-spacing-x:0;--tw-border-spacing-y:0;--tw-brightness:;--tw-contrast:;--tw-drop-shadow:;--tw-gradient-from-position:;--tw-gradient-to-position:;--tw-gradient-via-position:;--tw-grayscale:;--tw-hue-rotate:;--tw-invert:;--tw-numeric-figure:;--tw-numeric-fraction:;--tw-numeric-spacing:;--tw-ordinal:;--tw-pan-x:;--tw-pan-y:;--tw-pinch-zoom:;--tw-ring-color:rgba(69,89,164,.5);--tw-ring-inset:;--tw-ring-offset-color:#fff;--tw-ring-offset-shadow:0 0 transparent;--tw-ring-offset-width:0px;--tw-ring-shadow:0 0 transparent;--tw-rotate:0;--tw-saturate:;--tw-scale-x:1;--tw-scale-y:1;--tw-scroll-snap-strictness:proximity;--tw-sepia:;--tw-shadow-colored:0 0 transparent;--tw-shadow:0 0 transparent;--tw-skew-x:0;--tw-skew-y:0;--tw-slashed-zero:;--tw-translate-x:0;--tw-translate-y:0;-webkit-text-stroke-width:0px;background-color:rgb(255, 255, 255);border:0px solid rgb(227, 227, 227);box-sizing:border-box;color:rgb(13, 13, 13);font-family:Söhne, ui-sans-serif, system-ui, -apple-system, &amp;quot;Segoe UI&amp;quot;, Roboto, Ubuntu, Cantarell, &amp;quot;Noto Sans&amp;quot;, sans-serif, &amp;quot;Helvetica Neue&amp;quot;, Arial, &amp;quot;Apple Color Emoji&amp;quot;, &amp;quot;Segoe UI Emoji&amp;quot;, &amp;quot;Segoe UI Symbol&amp;quot;, &amp;quot;Noto Color Emoji&amp;quot;;font-size:16px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:normal;margin:1.25em 0px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;🏡 Địa chỉ: 14/2 Gio An - P.5 - TP.Đà Lạt&amp;nbsp;&lt;/p&gt;&lt;p style="--tw-backdrop-blur:;--tw-backdrop-brightness:;--tw-backdrop-contrast:;--tw-backdrop-grayscale:;--tw-backdrop-hue-rotate:;--tw-backdrop-invert:;--tw-backdrop-opacity:;--tw-backdrop-saturate:;--tw-backdrop-sepia:;--tw-blur:;--tw-border-spacing-x:0;--tw-border-spacing-y:0;--tw-brightness:;--tw-contrast:;--tw-drop-shadow:;--tw-gradient-from-position:;--tw-gradient-to-position:;--tw-gradient-via-position:;--tw-grayscale:;--tw-hue-rotate:;--tw-invert:;--tw-numeric-figure:;--tw-numeric-fraction:;--tw-numeric-spacing:;--tw-ordinal:;--tw-pan-x:;--tw-pan-y:;--tw-pinch-zoom:;--tw-ring-color:rgba(69,89,164,.5);--tw-ring-inset:;--tw-ring-offset-color:#fff;--tw-ring-offset-shadow:0 0 transparent;--tw-ring-offset-width:0px;--tw-ring-shadow:0 0 transparent;--tw-rotate:0;--tw-saturate:;--tw-scale-x:1;--tw-scale-y:1;--tw-scroll-snap-strictness:proximity;--tw-sepia:;--tw-shadow-colored:0 0 transparent;--tw-shadow:0 0 transparent;--tw-skew-x:0;--tw-skew-y:0;--tw-slashed-zero:;--tw-translate-x:0;--tw-translate-y:0;-webkit-text-stroke-width:0px;background-color:rgb(255, 255, 255);border:0px solid rgb(227, 227, 227);box-sizing:border-box;color:rgb(13, 13, 13);font-family:Söhne, ui-sans-serif, system-ui, -apple-system, &amp;quot;Segoe UI&amp;quot;, Roboto, Ubuntu, Cantarell, &amp;quot;Noto Sans&amp;quot;, sans-serif, &amp;quot;Helvetica Neue&amp;quot;, Arial, &amp;quot;Apple Color Emoji&amp;quot;, &amp;quot;Segoe UI Emoji&amp;quot;, &amp;quot;Segoe UI Symbol&amp;quot;, &amp;quot;Noto Color Emoji&amp;quot;;font-size:16px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:normal;margin:1.25em 0px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;🛵 Chỉ cách trung tâm 5 phút đi xe máy.&lt;/p&gt;&lt;p style="--tw-backdrop-blur:;--tw-backdrop-brightness:;--tw-backdrop-contrast:;--tw-backdrop-grayscale:;--tw-backdrop-hue-rotate:;--tw-backdrop-invert:;--tw-backdrop-opacity:;--tw-backdrop-saturate:;--tw-backdrop-sepia:;--tw-blur:;--tw-border-spacing-x:0;--tw-border-spacing-y:0;--tw-brightness:;--tw-contrast:;--tw-drop-shadow:;--tw-gradient-from-position:;--tw-gradient-to-position:;--tw-gradient-via-position:;--tw-grayscale:;--tw-hue-rotate:;--tw-invert:;--tw-numeric-figure:;--tw-numeric-fraction:;--tw-numeric-spacing:;--tw-ordinal:;--tw-pan-x:;--tw-pan-y:;--tw-pinch-zoom:;--tw-ring-color:rgba(69,89,164,.5);--tw-ring-inset:;--tw-ring-offset-color:#fff;--tw-ring-offset-shadow:0 0 transparent;--tw-ring-offset-width:0px;--tw-ring-shadow:0 0 transparent;--tw-rotate:0;--tw-saturate:;--tw-scale-x:1;--tw-scale-y:1;--tw-scroll-snap-strictness:proximity;--tw-sepia:;--tw-shadow-colored:0 0 transparent;--tw-shadow:0 0 transparent;--tw-skew-x:0;--tw-skew-y:0;--tw-slashed-zero:;--tw-translate-x:0;--tw-translate-y:0;-webkit-text-stroke-width:0px;background-color:rgb(255, 255, 255);border:0px solid rgb(227, 227, 227);box-sizing:border-box;color:rgb(13, 13, 13);font-family:Söhne, ui-sans-serif, system-ui, -apple-system, &amp;quot;Segoe UI&amp;quot;, Roboto, Ubuntu, Cantarell, &amp;quot;Noto Sans&amp;quot;, sans-serif, &amp;quot;Helvetica Neue&amp;quot;, Arial, &amp;quot;Apple Color Emoji&amp;quot;, &amp;quot;Segoe UI Emoji&amp;quot;, &amp;quot;Segoe UI Symbol&amp;quot;, &amp;quot;Noto Color Emoji&amp;quot;;font-size:16px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:normal;margin:1.25em 0px 0px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;Homestay Đà Lạt HS3 không chỉ là nơi dừng chân lý tưởng, mà còn là điểm đến tuyệt vời để bạn tận hưởng những khoảnh khắc thư giãn và đắm chìm trong không gian bình yên của Đà Lạt. Hãy đặt phòng ngay hôm nay để có một trải nghiệm đáng nhớ nhất! 🌲🌲🌲&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>SC23</t>
+  </si>
+  <si>
+    <t>Villa Đà Lạt SC23 - Villa mới toanh theo phong cách hiện đại, sang trọng.</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>Địa chỉ: 91 Hùng Vương - Khu Du lịch Nam Hồ Phường 11 - TP. Đà Lạt</t>
+  </si>
+  <si>
+    <t>&lt;p&gt;&lt;span style="background-color:rgb(255,255,255);color:rgb(8,28,54);font-family:SegoeuiPc, &amp;quot;Segoe UI&amp;quot;, &amp;quot;San Francisco&amp;quot;, &amp;quot;Helvetica Neue&amp;quot;, Helvetica, &amp;quot;Lucida Grande&amp;quot;, Roboto, Ubuntu, Tahoma, &amp;quot;Microsoft Sans Serif&amp;quot;, Arial, sans-serif;font-size:15px;"&gt;&lt;span class="text" style="-webkit-text-stroke-width:0px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:0.2px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;user-select:text;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;Villa Đà Lạt SC23 - Villa mới toanh theo phong cách hiện đại, sang trọng. Nằm trong KDL Biệt thự nghĩ dưỡng Nam Hồ-Khu vực đặc biệt an ninh và yên tĩnh. Cách chợ Đà Lạt 5km với 5-7 phút di chuyển ra trung tâm.&amp;nbsp;&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color:rgb(255,255,255);color:rgb(8,28,54);font-family:SegoeuiPc, &amp;quot;Segoe UI&amp;quot;, &amp;quot;San Francisco&amp;quot;, &amp;quot;Helvetica Neue&amp;quot;, Helvetica, &amp;quot;Lucida Grande&amp;quot;, Roboto, Ubuntu, Tahoma, &amp;quot;Microsoft Sans Serif&amp;quot;, Arial, sans-serif;font-size:15px;"&gt;&lt;span class="text" style="-webkit-text-stroke-width:0px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:0.2px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;user-select:text;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;Cơ cấu: &lt;/span&gt;&lt;/span&gt;&lt;span style="background-color:rgb(255,255,255);color:transparent;font-family:SegoeuiPc, &amp;quot;Segoe UI&amp;quot;, &amp;quot;San Francisco&amp;quot;, &amp;quot;Helvetica Neue&amp;quot;, Helvetica, &amp;quot;Lucida Grande&amp;quot;, Roboto, Ubuntu, Tahoma, &amp;quot;Microsoft Sans Serif&amp;quot;, Arial, sans-serif;font-size:15px;"&gt;&lt;span class="emoji-sizer emoji-outer " style="-webkit-text-stroke-width:0px;-webkit-user-drag:element;background-image:url(&amp;quot;emoji/emoji-40/row-14-column-33.png&amp;quot;);background-repeat:no-repeat;background-size:contain;display:inline-block;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;height:22px;letter-spacing:50px;margin:0px 0px -3px;orphans:2;overflow:hidden;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-shadow:none;text-transform:none;white-space:normal;widows:2;width:22px;word-spacing:0px;"&gt;?&lt;/span&gt;&lt;/span&gt;&lt;span style="background-color:rgb(255,255,255);color:rgb(8,28,54);font-family:SegoeuiPc, &amp;quot;Segoe UI&amp;quot;, &amp;quot;San Francisco&amp;quot;, &amp;quot;Helvetica Neue&amp;quot;, Helvetica, &amp;quot;Lucida Grande&amp;quot;, Roboto, Ubuntu, Tahoma, &amp;quot;Microsoft Sans Serif&amp;quot;, Arial, sans-serif;font-size:15px;"&gt;&lt;span class="text" style="-webkit-text-stroke-width:0px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:0.2px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;user-select:text;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;&amp;nbsp;&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color:rgb(255,255,255);color:rgb(8,28,54);font-family:SegoeuiPc, &amp;quot;Segoe UI&amp;quot;, &amp;quot;San Francisco&amp;quot;, &amp;quot;Helvetica Neue&amp;quot;, Helvetica, &amp;quot;Lucida Grande&amp;quot;, Roboto, Ubuntu, Tahoma, &amp;quot;Microsoft Sans Serif&amp;quot;, Arial, sans-serif;font-size:15px;"&gt;&lt;span class="text" style="-webkit-text-stroke-width:0px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:0.2px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;user-select:text;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;Gồm 4 phòng ngủ: 3 Phòng 1 giường (1m8) và 1 phòng 2 giường (1m6) - 5wc Villa có trang bị thêm nệm dự phòng. Sức chứa 12-15 Khách. &lt;/span&gt;&lt;/span&gt;&lt;span style="background-color:rgb(255,255,255);color:transparent;font-family:SegoeuiPc, &amp;quot;Segoe UI&amp;quot;, &amp;quot;San Francisco&amp;quot;, &amp;quot;Helvetica Neue&amp;quot;, Helvetica, &amp;quot;Lucida Grande&amp;quot;, Roboto, Ubuntu, Tahoma, &amp;quot;Microsoft Sans Serif&amp;quot;, Arial, sans-serif;font-size:15px;"&gt;&lt;span class="emoji-sizer emoji-outer " style="-webkit-text-stroke-width:0px;-webkit-user-drag:element;background-image:url(&amp;quot;emoji/emoji-40/row-14-column-33.png&amp;quot;);background-repeat:no-repeat;background-size:contain;display:inline-block;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;height:22px;letter-spacing:50px;margin:0px 0px -3px;orphans:2;overflow:hidden;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-shadow:none;text-transform:none;white-space:normal;widows:2;width:22px;word-spacing:0px;"&gt;?&lt;/span&gt;&lt;/span&gt;&lt;span style="background-color:rgb(255,255,255);color:rgb(8,28,54);font-family:SegoeuiPc, &amp;quot;Segoe UI&amp;quot;, &amp;quot;San Francisco&amp;quot;, &amp;quot;Helvetica Neue&amp;quot;, Helvetica, &amp;quot;Lucida Grande&amp;quot;, Roboto, Ubuntu, Tahoma, &amp;quot;Microsoft Sans Serif&amp;quot;, Arial, sans-serif;font-size:15px;"&gt;&lt;span class="text" style="-webkit-text-stroke-width:0px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:0.2px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;user-select:text;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;&amp;nbsp;&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color:rgb(255,255,255);color:rgb(8,28,54);font-family:SegoeuiPc, &amp;quot;Segoe UI&amp;quot;, &amp;quot;San Francisco&amp;quot;, &amp;quot;Helvetica Neue&amp;quot;, Helvetica, &amp;quot;Lucida Grande&amp;quot;, Roboto, Ubuntu, Tahoma, &amp;quot;Microsoft Sans Serif&amp;quot;, Arial, sans-serif;font-size:15px;"&gt;&lt;span class="text" style="-webkit-text-stroke-width:0px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:0.2px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;user-select:text;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;01 Phòng khách , 01 phòng bếp đầy đủ tiện nghi. &lt;/span&gt;&lt;/span&gt;&lt;span style="background-color:rgb(255,255,255);color:transparent;font-family:SegoeuiPc, &amp;quot;Segoe UI&amp;quot;, &amp;quot;San Francisco&amp;quot;, &amp;quot;Helvetica Neue&amp;quot;, Helvetica, &amp;quot;Lucida Grande&amp;quot;, Roboto, Ubuntu, Tahoma, &amp;quot;Microsoft Sans Serif&amp;quot;, Arial, sans-serif;font-size:15px;"&gt;&lt;span class="emoji-sizer emoji-outer " style="-webkit-text-stroke-width:0px;-webkit-user-drag:element;background-image:url(&amp;quot;emoji/emoji-40/row-14-column-33.png&amp;quot;);background-repeat:no-repeat;background-size:contain;display:inline-block;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;height:22px;letter-spacing:50px;margin:0px 0px -3px;orphans:2;overflow:hidden;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-shadow:none;text-transform:none;white-space:normal;widows:2;width:22px;word-spacing:0px;"&gt;?&lt;/span&gt;&lt;/span&gt;&lt;span style="background-color:rgb(255,255,255);color:rgb(8,28,54);font-family:SegoeuiPc, &amp;quot;Segoe UI&amp;quot;, &amp;quot;San Francisco&amp;quot;, &amp;quot;Helvetica Neue&amp;quot;, Helvetica, &amp;quot;Lucida Grande&amp;quot;, Roboto, Ubuntu, Tahoma, &amp;quot;Microsoft Sans Serif&amp;quot;, Arial, sans-serif;font-size:15px;"&gt;&lt;span class="text" style="-webkit-text-stroke-width:0px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:0.2px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;user-select:text;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;&amp;nbsp;&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color:rgb(255,255,255);color:rgb(8,28,54);font-family:SegoeuiPc, &amp;quot;Segoe UI&amp;quot;, &amp;quot;San Francisco&amp;quot;, &amp;quot;Helvetica Neue&amp;quot;, Helvetica, &amp;quot;Lucida Grande&amp;quot;, Roboto, Ubuntu, Tahoma, &amp;quot;Microsoft Sans Serif&amp;quot;, Arial, sans-serif;font-size:15px;"&gt;&lt;span class="text" style="-webkit-text-stroke-width:0px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:0.2px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;user-select:text;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;Sân vườn rộng rãi tiêu chuẩn thích hợp cho BBQ. Đậu xe trong khuôn viên.&amp;nbsp;&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;</t>
+  </si>
+  <si>
+    <t>SC27</t>
+  </si>
+  <si>
+    <t>Villa Đà Lạt SC27 - Không gian yên tĩnh trong lành, đặc trưng khí hậu Đà Lạt rất thích hợp nghĩ dưỡng.</t>
+  </si>
+  <si>
+    <t>Địa chỉ :Toạ lạc tại đường Hùng Vương cách chợ khoảng 5km với 7-10 phút chạy xe</t>
+  </si>
+  <si>
     <t>VILLA BÌNH DÂN</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&amp;nbsp;&lt;span style="background-color:rgb(255,255,255);color:rgb(13,13,13);font-family:Söhne, ui-sans-serif, system-ui, -apple-system, &amp;quot;Segoe UI&amp;quot;, Roboto, Ubuntu, Cantarell, &amp;quot;Noto Sans&amp;quot;, sans-serif, &amp;quot;Helvetica Neue&amp;quot;, Arial, &amp;quot;Apple Color Emoji&amp;quot;, &amp;quot;Segoe UI Emoji&amp;quot;, &amp;quot;Segoe UI Symbol&amp;quot;, &amp;quot;Noto Color Emoji&amp;quot;;font-size:16px;"&gt;&lt;span style="-webkit-text-stroke-width:0px;display:inline !important;float:none;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:normal;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;Dạo này, mọi người đang cảm thấy mệt mỏi với nhịp sống hối hả và tiêu cực? Đừng lo lắng nữa! Hãy để Homestay Đà Lạt HS3 là điểm dừng chân lý tưởng của bạn để tìm lại sự bình yên và hạnh phúc!&amp;nbsp;&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;&lt;p style="--tw-backdrop-blur:;--tw-backdrop-brightness:;--tw-backdrop-contrast:;--tw-backdrop-grayscale:;--tw-backdrop-hue-rotate:;--tw-backdrop-invert:;--tw-backdrop-opacity:;--tw-backdrop-saturate:;--tw-backdrop-sepia:;--tw-blur:;--tw-border-spacing-x:0;--tw-border-spacing-y:0;--tw-brightness:;--tw-contrast:;--tw-drop-shadow:;--tw-gradient-from-position:;--tw-gradient-to-position:;--tw-gradient-via-position:;--tw-grayscale:;--tw-hue-rotate:;--tw-invert:;--tw-numeric-figure:;--tw-numeric-fraction:;--tw-numeric-spacing:;--tw-ordinal:;--tw-pan-x:;--tw-pan-y:;--tw-pinch-zoom:;--tw-ring-color:rgba(69,89,164,.5);--tw-ring-inset:;--tw-ring-offset-color:#fff;--tw-ring-offset-shadow:0 0 transparent;--tw-ring-offset-width:0px;--tw-ring-shadow:0 0 transparent;--tw-rotate:0;--tw-saturate:;--tw-scale-x:1;--tw-scale-y:1;--tw-scroll-snap-strictness:proximity;--tw-sepia:;--tw-shadow-colored:0 0 transparent;--tw-shadow:0 0 transparent;--tw-skew-x:0;--tw-skew-y:0;--tw-slashed-zero:;--tw-translate-x:0;--tw-translate-y:0;-webkit-text-stroke-width:0px;background-color:rgb(255, 255, 255);border:0px solid rgb(227, 227, 227);box-sizing:border-box;color:rgb(13, 13, 13);font-family:Söhne, ui-sans-serif, system-ui, -apple-system, &amp;quot;Segoe UI&amp;quot;, Roboto, Ubuntu, Cantarell, &amp;quot;Noto Sans&amp;quot;, sans-serif, &amp;quot;Helvetica Neue&amp;quot;, Arial, &amp;quot;Apple Color Emoji&amp;quot;, &amp;quot;Segoe UI Emoji&amp;quot;, &amp;quot;Segoe UI Symbol&amp;quot;, &amp;quot;Noto Color Emoji&amp;quot;;font-size:16px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:normal;margin:1.25em 0px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;📌 Cơ cấu: 3 phòng ngủ - 3 toilet, thiết kế sang trọng và ấm cúng.&amp;nbsp;&lt;/p&gt;&lt;p style="--tw-backdrop-blur:;--tw-backdrop-brightness:;--tw-backdrop-contrast:;--tw-backdrop-grayscale:;--tw-backdrop-hue-rotate:;--tw-backdrop-invert:;--tw-backdrop-opacity:;--tw-backdrop-saturate:;--tw-backdrop-sepia:;--tw-blur:;--tw-border-spacing-x:0;--tw-border-spacing-y:0;--tw-brightness:;--tw-contrast:;--tw-drop-shadow:;--tw-gradient-from-position:;--tw-gradient-to-position:;--tw-gradient-via-position:;--tw-grayscale:;--tw-hue-rotate:;--tw-invert:;--tw-numeric-figure:;--tw-numeric-fraction:;--tw-numeric-spacing:;--tw-ordinal:;--tw-pan-x:;--tw-pan-y:;--tw-pinch-zoom:;--tw-ring-color:rgba(69,89,164,.5);--tw-ring-inset:;--tw-ring-offset-color:#fff;--tw-ring-offset-shadow:0 0 transparent;--tw-ring-offset-width:0px;--tw-ring-shadow:0 0 transparent;--tw-rotate:0;--tw-saturate:;--tw-scale-x:1;--tw-scale-y:1;--tw-scroll-snap-strictness:proximity;--tw-sepia:;--tw-shadow-colored:0 0 transparent;--tw-shadow:0 0 transparent;--tw-skew-x:0;--tw-skew-y:0;--tw-slashed-zero:;--tw-translate-x:0;--tw-translate-y:0;-webkit-text-stroke-width:0px;background-color:rgb(255, 255, 255);border:0px solid rgb(227, 227, 227);box-sizing:border-box;color:rgb(13, 13, 13);font-family:Söhne, ui-sans-serif, system-ui, -apple-system, &amp;quot;Segoe UI&amp;quot;, Roboto, Ubuntu, Cantarell, &amp;quot;Noto Sans&amp;quot;, sans-serif, &amp;quot;Helvetica Neue&amp;quot;, Arial, &amp;quot;Apple Color Emoji&amp;quot;, &amp;quot;Segoe UI Emoji&amp;quot;, &amp;quot;Segoe UI Symbol&amp;quot;, &amp;quot;Noto Color Emoji&amp;quot;;font-size:16px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:normal;margin:1.25em 0px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;👩‍🍳 Bếp Ngọt Ngào: Không gian bếp ấm áp với những dụng cụ nấu nướng đầy đủ, cho bạn tự do sáng tạo và thưởng thức những món ngon.&lt;/p&gt;&lt;p style="--tw-backdrop-blur:;--tw-backdrop-brightness:;--tw-backdrop-contrast:;--tw-backdrop-grayscale:;--tw-backdrop-hue-rotate:;--tw-backdrop-invert:;--tw-backdrop-opacity:;--tw-backdrop-saturate:;--tw-backdrop-sepia:;--tw-blur:;--tw-border-spacing-x:0;--tw-border-spacing-y:0;--tw-brightness:;--tw-contrast:;--tw-drop-shadow:;--tw-gradient-from-position:;--tw-gradient-to-position:;--tw-gradient-via-position:;--tw-grayscale:;--tw-hue-rotate:;--tw-invert:;--tw-numeric-figure:;--tw-numeric-fraction:;--tw-numeric-spacing:;--tw-ordinal:;--tw-pan-x:;--tw-pan-y:;--tw-pinch-zoom:;--tw-ring-color:rgba(69,89,164,.5);--tw-ring-inset:;--tw-ring-offset-color:#fff;--tw-ring-offset-shadow:0 0 transparent;--tw-ring-offset-width:0px;--tw-ring-shadow:0 0 transparent;--tw-rotate:0;--tw-saturate:;--tw-scale-x:1;--tw-scale-y:1;--tw-scroll-snap-strictness:proximity;--tw-sepia:;--tw-shadow-colored:0 0 transparent;--tw-shadow:0 0 transparent;--tw-skew-x:0;--tw-skew-y:0;--tw-slashed-zero:;--tw-translate-x:0;--tw-translate-y:0;-webkit-text-stroke-width:0px;background-color:rgb(255, 255, 255);border:0px solid rgb(227, 227, 227);box-sizing:border-box;color:rgb(13, 13, 13);font-family:Söhne, ui-sans-serif, system-ui, -apple-system, &amp;quot;Segoe UI&amp;quot;, Roboto, Ubuntu, Cantarell, &amp;quot;Noto Sans&amp;quot;, sans-serif, &amp;quot;Helvetica Neue&amp;quot;, Arial, &amp;quot;Apple Color Emoji&amp;quot;, &amp;quot;Segoe UI Emoji&amp;quot;, &amp;quot;Segoe UI Symbol&amp;quot;, &amp;quot;Noto Color Emoji&amp;quot;;font-size:16px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:normal;margin:1.25em 0px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;&amp;nbsp;🫶🏻 Sân BBQ : Sân BBQ thoáng đãng, là nơi lý tưởng cho các buổi tiệc nướng vui vẻ và đầy ấm áp.&amp;nbsp;&lt;/p&gt;&lt;p style="--tw-backdrop-blur:;--tw-backdrop-brightness:;--tw-backdrop-contrast:;--tw-backdrop-grayscale:;--tw-backdrop-hue-rotate:;--tw-backdrop-invert:;--tw-backdrop-opacity:;--tw-backdrop-saturate:;--tw-backdrop-sepia:;--tw-blur:;--tw-border-spacing-x:0;--tw-border-spacing-y:0;--tw-brightness:;--tw-contrast:;--tw-drop-shadow:;--tw-gradient-from-position:;--tw-gradient-to-position:;--tw-gradient-via-position:;--tw-grayscale:;--tw-hue-rotate:;--tw-invert:;--tw-numeric-figure:;--tw-numeric-fraction:;--tw-numeric-spacing:;--tw-ordinal:;--tw-pan-x:;--tw-pan-y:;--tw-pinch-zoom:;--tw-ring-color:rgba(69,89,164,.5);--tw-ring-inset:;--tw-ring-offset-color:#fff;--tw-ring-offset-shadow:0 0 transparent;--tw-ring-offset-width:0px;--tw-ring-shadow:0 0 transparent;--tw-rotate:0;--tw-saturate:;--tw-scale-x:1;--tw-scale-y:1;--tw-scroll-snap-strictness:proximity;--tw-sepia:;--tw-shadow-colored:0 0 transparent;--tw-shadow:0 0 transparent;--tw-skew-x:0;--tw-skew-y:0;--tw-slashed-zero:;--tw-translate-x:0;--tw-translate-y:0;-webkit-text-stroke-width:0px;background-color:rgb(255, 255, 255);border:0px solid rgb(227, 227, 227);box-sizing:border-box;color:rgb(13, 13, 13);font-family:Söhne, ui-sans-serif, system-ui, -apple-system, &amp;quot;Segoe UI&amp;quot;, Roboto, Ubuntu, Cantarell, &amp;quot;Noto Sans&amp;quot;, sans-serif, &amp;quot;Helvetica Neue&amp;quot;, Arial, &amp;quot;Apple Color Emoji&amp;quot;, &amp;quot;Segoe UI Emoji&amp;quot;, &amp;quot;Segoe UI Symbol&amp;quot;, &amp;quot;Noto Color Emoji&amp;quot;;font-size:16px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:normal;margin:1.25em 0px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;📌 Máy Nước Nóng: Sẵn có nước nóng 24/7, đảm bảo bạn luôn cảm thấy thoải mái và thư giãn.&amp;nbsp;&lt;/p&gt;&lt;p style="--tw-backdrop-blur:;--tw-backdrop-brightness:;--tw-backdrop-contrast:;--tw-backdrop-grayscale:;--tw-backdrop-hue-rotate:;--tw-backdrop-invert:;--tw-backdrop-opacity:;--tw-backdrop-saturate:;--tw-backdrop-sepia:;--tw-blur:;--tw-border-spacing-x:0;--tw-border-spacing-y:0;--tw-brightness:;--tw-contrast:;--tw-drop-shadow:;--tw-gradient-from-position:;--tw-gradient-to-position:;--tw-gradient-via-position:;--tw-grayscale:;--tw-hue-rotate:;--tw-invert:;--tw-numeric-figure:;--tw-numeric-fraction:;--tw-numeric-spacing:;--tw-ordinal:;--tw-pan-x:;--tw-pan-y:;--tw-pinch-zoom:;--tw-ring-color:rgba(69,89,164,.5);--tw-ring-inset:;--tw-ring-offset-color:#fff;--tw-ring-offset-shadow:0 0 transparent;--tw-ring-offset-width:0px;--tw-ring-shadow:0 0 transparent;--tw-rotate:0;--tw-saturate:;--tw-scale-x:1;--tw-scale-y:1;--tw-scroll-snap-strictness:proximity;--tw-sepia:;--tw-shadow-colored:0 0 transparent;--tw-shadow:0 0 transparent;--tw-skew-x:0;--tw-skew-y:0;--tw-slashed-zero:;--tw-translate-x:0;--tw-translate-y:0;-webkit-text-stroke-width:0px;background-color:rgb(255, 255, 255);border:0px solid rgb(227, 227, 227);box-sizing:border-box;color:rgb(13, 13, 13);font-family:Söhne, ui-sans-serif, system-ui, -apple-system, &amp;quot;Segoe UI&amp;quot;, Roboto, Ubuntu, Cantarell, &amp;quot;Noto Sans&amp;quot;, sans-serif, &amp;quot;Helvetica Neue&amp;quot;, Arial, &amp;quot;Apple Color Emoji&amp;quot;, &amp;quot;Segoe UI Emoji&amp;quot;, &amp;quot;Segoe UI Symbol&amp;quot;, &amp;quot;Noto Color Emoji&amp;quot;;font-size:16px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:normal;margin:1.25em 0px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;📌 Đèn Chiếu Sáng: Hãy thư giãn dưới ánh đèn màu vàng ấm áp, tạo không gian lý tưởng cho việc đọc sách và tận hưởng khoảnh khắc riêng tư.&amp;nbsp;&lt;/p&gt;&lt;p style="--tw-backdrop-blur:;--tw-backdrop-brightness:;--tw-backdrop-contrast:;--tw-backdrop-grayscale:;--tw-backdrop-hue-rotate:;--tw-backdrop-invert:;--tw-backdrop-opacity:;--tw-backdrop-saturate:;--tw-backdrop-sepia:;--tw-blur:;--tw-border-spacing-x:0;--tw-border-spacing-y:0;--tw-brightness:;--tw-contrast:;--tw-drop-shadow:;--tw-gradient-from-position:;--tw-gradient-to-position:;--tw-gradient-via-position:;--tw-grayscale:;--tw-hue-rotate:;--tw-invert:;--tw-numeric-figure:;--tw-numeric-fraction:;--tw-numeric-spacing:;--tw-ordinal:;--tw-pan-x:;--tw-pan-y:;--tw-pinch-zoom:;--tw-ring-color:rgba(69,89,164,.5);--tw-ring-inset:;--tw-ring-offset-color:#fff;--tw-ring-offset-shadow:0 0 transparent;--tw-ring-offset-width:0px;--tw-ring-shadow:0 0 transparent;--tw-rotate:0;--tw-saturate:;--tw-scale-x:1;--tw-scale-y:1;--tw-scroll-snap-strictness:proximity;--tw-sepia:;--tw-shadow-colored:0 0 transparent;--tw-shadow:0 0 transparent;--tw-skew-x:0;--tw-skew-y:0;--tw-slashed-zero:;--tw-translate-x:0;--tw-translate-y:0;-webkit-text-stroke-width:0px;background-color:rgb(255, 255, 255);border:0px solid rgb(227, 227, 227);box-sizing:border-box;color:rgb(13, 13, 13);font-family:Söhne, ui-sans-serif, system-ui, -apple-system, &amp;quot;Segoe UI&amp;quot;, Roboto, Ubuntu, Cantarell, &amp;quot;Noto Sans&amp;quot;, sans-serif, &amp;quot;Helvetica Neue&amp;quot;, Arial, &amp;quot;Apple Color Emoji&amp;quot;, &amp;quot;Segoe UI Emoji&amp;quot;, &amp;quot;Segoe UI Symbol&amp;quot;, &amp;quot;Noto Color Emoji&amp;quot;;font-size:16px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:normal;margin:1.25em 0px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;🏡 Địa chỉ: 14/2 Gio An - P.5 - TP.Đà Lạt&amp;nbsp;&lt;/p&gt;&lt;p style="--tw-backdrop-blur:;--tw-backdrop-brightness:;--tw-backdrop-contrast:;--tw-backdrop-grayscale:;--tw-backdrop-hue-rotate:;--tw-backdrop-invert:;--tw-backdrop-opacity:;--tw-backdrop-saturate:;--tw-backdrop-sepia:;--tw-blur:;--tw-border-spacing-x:0;--tw-border-spacing-y:0;--tw-brightness:;--tw-contrast:;--tw-drop-shadow:;--tw-gradient-from-position:;--tw-gradient-to-position:;--tw-gradient-via-position:;--tw-grayscale:;--tw-hue-rotate:;--tw-invert:;--tw-numeric-figure:;--tw-numeric-fraction:;--tw-numeric-spacing:;--tw-ordinal:;--tw-pan-x:;--tw-pan-y:;--tw-pinch-zoom:;--tw-ring-color:rgba(69,89,164,.5);--tw-ring-inset:;--tw-ring-offset-color:#fff;--tw-ring-offset-shadow:0 0 transparent;--tw-ring-offset-width:0px;--tw-ring-shadow:0 0 transparent;--tw-rotate:0;--tw-saturate:;--tw-scale-x:1;--tw-scale-y:1;--tw-scroll-snap-strictness:proximity;--tw-sepia:;--tw-shadow-colored:0 0 transparent;--tw-shadow:0 0 transparent;--tw-skew-x:0;--tw-skew-y:0;--tw-slashed-zero:;--tw-translate-x:0;--tw-translate-y:0;-webkit-text-stroke-width:0px;background-color:rgb(255, 255, 255);border:0px solid rgb(227, 227, 227);box-sizing:border-box;color:rgb(13, 13, 13);font-family:Söhne, ui-sans-serif, system-ui, -apple-system, &amp;quot;Segoe UI&amp;quot;, Roboto, Ubuntu, Cantarell, &amp;quot;Noto Sans&amp;quot;, sans-serif, &amp;quot;Helvetica Neue&amp;quot;, Arial, &amp;quot;Apple Color Emoji&amp;quot;, &amp;quot;Segoe UI Emoji&amp;quot;, &amp;quot;Segoe UI Symbol&amp;quot;, &amp;quot;Noto Color Emoji&amp;quot;;font-size:16px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:normal;margin:1.25em 0px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;🛵 Chỉ cách trung tâm 5 phút đi xe máy.&lt;/p&gt;&lt;p style="--tw-backdrop-blur:;--tw-backdrop-brightness:;--tw-backdrop-contrast:;--tw-backdrop-grayscale:;--tw-backdrop-hue-rotate:;--tw-backdrop-invert:;--tw-backdrop-opacity:;--tw-backdrop-saturate:;--tw-backdrop-sepia:;--tw-blur:;--tw-border-spacing-x:0;--tw-border-spacing-y:0;--tw-brightness:;--tw-contrast:;--tw-drop-shadow:;--tw-gradient-from-position:;--tw-gradient-to-position:;--tw-gradient-via-position:;--tw-grayscale:;--tw-hue-rotate:;--tw-invert:;--tw-numeric-figure:;--tw-numeric-fraction:;--tw-numeric-spacing:;--tw-ordinal:;--tw-pan-x:;--tw-pan-y:;--tw-pinch-zoom:;--tw-ring-color:rgba(69,89,164,.5);--tw-ring-inset:;--tw-ring-offset-color:#fff;--tw-ring-offset-shadow:0 0 transparent;--tw-ring-offset-width:0px;--tw-ring-shadow:0 0 transparent;--tw-rotate:0;--tw-saturate:;--tw-scale-x:1;--tw-scale-y:1;--tw-scroll-snap-strictness:proximity;--tw-sepia:;--tw-shadow-colored:0 0 transparent;--tw-shadow:0 0 transparent;--tw-skew-x:0;--tw-skew-y:0;--tw-slashed-zero:;--tw-translate-x:0;--tw-translate-y:0;-webkit-text-stroke-width:0px;background-color:rgb(255, 255, 255);border:0px solid rgb(227, 227, 227);box-sizing:border-box;color:rgb(13, 13, 13);font-family:Söhne, ui-sans-serif, system-ui, -apple-system, &amp;quot;Segoe UI&amp;quot;, Roboto, Ubuntu, Cantarell, &amp;quot;Noto Sans&amp;quot;, sans-serif, &amp;quot;Helvetica Neue&amp;quot;, Arial, &amp;quot;Apple Color Emoji&amp;quot;, &amp;quot;Segoe UI Emoji&amp;quot;, &amp;quot;Segoe UI Symbol&amp;quot;, &amp;quot;Noto Color Emoji&amp;quot;;font-size:16px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:normal;margin:1.25em 0px 0px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;Homestay Đà Lạt HS3 không chỉ là nơi dừng chân lý tưởng, mà còn là điểm đến tuyệt vời để bạn tận hưởng những khoảnh khắc thư giãn và đắm chìm trong không gian bình yên của Đà Lạt. Hãy đặt phòng ngay hôm nay để có một trải nghiệm đáng nhớ nhất! 🌲🌲🌲&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>SC23</t>
-  </si>
-  <si>
-    <t>Villa Đà Lạt SC23 - Villa mới toanh theo phong cách hiện đại, sang trọng.</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Địa chỉ: 91 Hùng Vương - Khu Du lịch Nam Hồ Phường 11 - TP. Đà Lạt</t>
-  </si>
-  <si>
-    <t>&lt;p&gt;&lt;span style="background-color:rgb(255,255,255);color:rgb(8,28,54);font-family:SegoeuiPc, &amp;quot;Segoe UI&amp;quot;, &amp;quot;San Francisco&amp;quot;, &amp;quot;Helvetica Neue&amp;quot;, Helvetica, &amp;quot;Lucida Grande&amp;quot;, Roboto, Ubuntu, Tahoma, &amp;quot;Microsoft Sans Serif&amp;quot;, Arial, sans-serif;font-size:15px;"&gt;&lt;span class="text" style="-webkit-text-stroke-width:0px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:0.2px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;user-select:text;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;Villa Đà Lạt SC23 - Villa mới toanh theo phong cách hiện đại, sang trọng. Nằm trong KDL Biệt thự nghĩ dưỡng Nam Hồ-Khu vực đặc biệt an ninh và yên tĩnh. Cách chợ Đà Lạt 5km với 5-7 phút di chuyển ra trung tâm.&amp;nbsp;&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color:rgb(255,255,255);color:rgb(8,28,54);font-family:SegoeuiPc, &amp;quot;Segoe UI&amp;quot;, &amp;quot;San Francisco&amp;quot;, &amp;quot;Helvetica Neue&amp;quot;, Helvetica, &amp;quot;Lucida Grande&amp;quot;, Roboto, Ubuntu, Tahoma, &amp;quot;Microsoft Sans Serif&amp;quot;, Arial, sans-serif;font-size:15px;"&gt;&lt;span class="text" style="-webkit-text-stroke-width:0px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:0.2px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;user-select:text;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;Cơ cấu: &lt;/span&gt;&lt;/span&gt;&lt;span style="background-color:rgb(255,255,255);color:transparent;font-family:SegoeuiPc, &amp;quot;Segoe UI&amp;quot;, &amp;quot;San Francisco&amp;quot;, &amp;quot;Helvetica Neue&amp;quot;, Helvetica, &amp;quot;Lucida Grande&amp;quot;, Roboto, Ubuntu, Tahoma, &amp;quot;Microsoft Sans Serif&amp;quot;, Arial, sans-serif;font-size:15px;"&gt;&lt;span class="emoji-sizer emoji-outer " style="-webkit-text-stroke-width:0px;-webkit-user-drag:element;background-image:url(&amp;quot;emoji/emoji-40/row-14-column-33.png&amp;quot;);background-repeat:no-repeat;background-size:contain;display:inline-block;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;height:22px;letter-spacing:50px;margin:0px 0px -3px;orphans:2;overflow:hidden;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-shadow:none;text-transform:none;white-space:normal;widows:2;width:22px;word-spacing:0px;"&gt;?&lt;/span&gt;&lt;/span&gt;&lt;span style="background-color:rgb(255,255,255);color:rgb(8,28,54);font-family:SegoeuiPc, &amp;quot;Segoe UI&amp;quot;, &amp;quot;San Francisco&amp;quot;, &amp;quot;Helvetica Neue&amp;quot;, Helvetica, &amp;quot;Lucida Grande&amp;quot;, Roboto, Ubuntu, Tahoma, &amp;quot;Microsoft Sans Serif&amp;quot;, Arial, sans-serif;font-size:15px;"&gt;&lt;span class="text" style="-webkit-text-stroke-width:0px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:0.2px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;user-select:text;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;&amp;nbsp;&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color:rgb(255,255,255);color:rgb(8,28,54);font-family:SegoeuiPc, &amp;quot;Segoe UI&amp;quot;, &amp;quot;San Francisco&amp;quot;, &amp;quot;Helvetica Neue&amp;quot;, Helvetica, &amp;quot;Lucida Grande&amp;quot;, Roboto, Ubuntu, Tahoma, &amp;quot;Microsoft Sans Serif&amp;quot;, Arial, sans-serif;font-size:15px;"&gt;&lt;span class="text" style="-webkit-text-stroke-width:0px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:0.2px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;user-select:text;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;Gồm 4 phòng ngủ: 3 Phòng 1 giường (1m8) và 1 phòng 2 giường (1m6) - 5wc Villa có trang bị thêm nệm dự phòng. Sức chứa 12-15 Khách. &lt;/span&gt;&lt;/span&gt;&lt;span style="background-color:rgb(255,255,255);color:transparent;font-family:SegoeuiPc, &amp;quot;Segoe UI&amp;quot;, &amp;quot;San Francisco&amp;quot;, &amp;quot;Helvetica Neue&amp;quot;, Helvetica, &amp;quot;Lucida Grande&amp;quot;, Roboto, Ubuntu, Tahoma, &amp;quot;Microsoft Sans Serif&amp;quot;, Arial, sans-serif;font-size:15px;"&gt;&lt;span class="emoji-sizer emoji-outer " style="-webkit-text-stroke-width:0px;-webkit-user-drag:element;background-image:url(&amp;quot;emoji/emoji-40/row-14-column-33.png&amp;quot;);background-repeat:no-repeat;background-size:contain;display:inline-block;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;height:22px;letter-spacing:50px;margin:0px 0px -3px;orphans:2;overflow:hidden;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-shadow:none;text-transform:none;white-space:normal;widows:2;width:22px;word-spacing:0px;"&gt;?&lt;/span&gt;&lt;/span&gt;&lt;span style="background-color:rgb(255,255,255);color:rgb(8,28,54);font-family:SegoeuiPc, &amp;quot;Segoe UI&amp;quot;, &amp;quot;San Francisco&amp;quot;, &amp;quot;Helvetica Neue&amp;quot;, Helvetica, &amp;quot;Lucida Grande&amp;quot;, Roboto, Ubuntu, Tahoma, &amp;quot;Microsoft Sans Serif&amp;quot;, Arial, sans-serif;font-size:15px;"&gt;&lt;span class="text" style="-webkit-text-stroke-width:0px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:0.2px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;user-select:text;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;&amp;nbsp;&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color:rgb(255,255,255);color:rgb(8,28,54);font-family:SegoeuiPc, &amp;quot;Segoe UI&amp;quot;, &amp;quot;San Francisco&amp;quot;, &amp;quot;Helvetica Neue&amp;quot;, Helvetica, &amp;quot;Lucida Grande&amp;quot;, Roboto, Ubuntu, Tahoma, &amp;quot;Microsoft Sans Serif&amp;quot;, Arial, sans-serif;font-size:15px;"&gt;&lt;span class="text" style="-webkit-text-stroke-width:0px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:0.2px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;user-select:text;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;01 Phòng khách , 01 phòng bếp đầy đủ tiện nghi. &lt;/span&gt;&lt;/span&gt;&lt;span style="background-color:rgb(255,255,255);color:transparent;font-family:SegoeuiPc, &amp;quot;Segoe UI&amp;quot;, &amp;quot;San Francisco&amp;quot;, &amp;quot;Helvetica Neue&amp;quot;, Helvetica, &amp;quot;Lucida Grande&amp;quot;, Roboto, Ubuntu, Tahoma, &amp;quot;Microsoft Sans Serif&amp;quot;, Arial, sans-serif;font-size:15px;"&gt;&lt;span class="emoji-sizer emoji-outer " style="-webkit-text-stroke-width:0px;-webkit-user-drag:element;background-image:url(&amp;quot;emoji/emoji-40/row-14-column-33.png&amp;quot;);background-repeat:no-repeat;background-size:contain;display:inline-block;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;height:22px;letter-spacing:50px;margin:0px 0px -3px;orphans:2;overflow:hidden;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-shadow:none;text-transform:none;white-space:normal;widows:2;width:22px;word-spacing:0px;"&gt;?&lt;/span&gt;&lt;/span&gt;&lt;span style="background-color:rgb(255,255,255);color:rgb(8,28,54);font-family:SegoeuiPc, &amp;quot;Segoe UI&amp;quot;, &amp;quot;San Francisco&amp;quot;, &amp;quot;Helvetica Neue&amp;quot;, Helvetica, &amp;quot;Lucida Grande&amp;quot;, Roboto, Ubuntu, Tahoma, &amp;quot;Microsoft Sans Serif&amp;quot;, Arial, sans-serif;font-size:15px;"&gt;&lt;span class="text" style="-webkit-text-stroke-width:0px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:0.2px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;user-select:text;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;&amp;nbsp;&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;&lt;p&gt;&lt;span style="background-color:rgb(255,255,255);color:rgb(8,28,54);font-family:SegoeuiPc, &amp;quot;Segoe UI&amp;quot;, &amp;quot;San Francisco&amp;quot;, &amp;quot;Helvetica Neue&amp;quot;, Helvetica, &amp;quot;Lucida Grande&amp;quot;, Roboto, Ubuntu, Tahoma, &amp;quot;Microsoft Sans Serif&amp;quot;, Arial, sans-serif;font-size:15px;"&gt;&lt;span class="text" style="-webkit-text-stroke-width:0px;font-style:normal;font-variant-caps:normal;font-variant-ligatures:normal;font-weight:400;letter-spacing:0.2px;orphans:2;text-align:start;text-decoration-color:initial;text-decoration-style:initial;text-decoration-thickness:initial;text-indent:0px;text-transform:none;user-select:text;white-space:pre-wrap;widows:2;word-spacing:0px;"&gt;Sân vườn rộng rãi tiêu chuẩn thích hợp cho BBQ. Đậu xe trong khuôn viên.&amp;nbsp;&lt;/span&gt;&lt;/span&gt;&lt;/p&gt;</t>
-  </si>
-  <si>
-    <t>SC27</t>
-  </si>
-  <si>
-    <t>Villa Đà Lạt SC27 - Không gian yên tĩnh trong lành, đặc trưng khí hậu Đà Lạt rất thích hợp nghĩ dưỡng.</t>
-  </si>
-  <si>
-    <t>Địa chỉ :Toạ lạc tại đường Hùng Vương cách chợ khoảng 5km với 7-10 phút chạy xe</t>
   </si>
   <si>
     <t>&lt;p&gt;Villa Đà Lạt SC27 - Chạm vào hương sắc tình khúc Đà Lạt, tôi ngất ngây.&lt;br&gt;Không gian yên tĩnh trong lành, đặc trưng khí hậu Đà Lạt rất thích hợp nghĩ dưỡng&lt;br&gt;Cơ cấu:&lt;br&gt;Có 3 phòng ngủ (2P đơn và 1P đôi).4wc.&lt;br&gt;Giao chìa khoá nguyên căn.&lt;/p&gt;&lt;p&gt;❇ Không gian yên tĩnh trong lành, đặc trưng khí hậu Đà Lạt rất thích hợp nghĩ dưỡng. &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp; &amp;nbsp;&amp;nbsp;&lt;br&gt;❇️ Sân vườn rộng, với những góc so chill cho những bữa tiệc BBQ quây quần bên gia đình.&lt;/p&gt;&lt;p&gt;❇Toạ lạc tại đường Hùng Vương cách chợ khoảng 5km với 7-10 phút chạy xe&lt;/p&gt;&lt;p&gt;? Chắc chắn là nơi nghỉ dưỡng du lịch lý tưởng cho du khách khi đến với thành phố hoa Đà Lạt&lt;/p&gt;</t>
@@ -264,7 +267,7 @@
     <col min="8" max="8" width="9.328125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="13.78125" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="5.45703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="15.546875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="17.66796875" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -404,10 +407,10 @@
         <v>1800000.0</v>
       </c>
       <c r="H4" t="n" s="0">
-        <v>45353.0</v>
+        <v>45358.0</v>
       </c>
       <c r="I4" t="n" s="0">
-        <v>45353.0</v>
+        <v>45358.0</v>
       </c>
       <c r="J4" t="n" s="0">
         <v>1.0</v>
@@ -489,10 +492,10 @@
         <v>1.0</v>
       </c>
       <c r="K6" t="s" s="0">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="L6" t="s" s="0">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="7">
@@ -500,10 +503,10 @@
         <v>7.0</v>
       </c>
       <c r="B7" t="s" s="0">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C7" t="s" s="0">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D7" t="s" s="0">
         <v>27</v>
@@ -512,7 +515,7 @@
         <v>33</v>
       </c>
       <c r="F7" t="s" s="0">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G7" t="n" s="0">
         <v>1000000.0</v>
@@ -527,10 +530,10 @@
         <v>1.0</v>
       </c>
       <c r="K7" t="s" s="0">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="L7" t="s" s="0">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8">
@@ -538,10 +541,10 @@
         <v>8.0</v>
       </c>
       <c r="B8" t="s" s="0">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s" s="0">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="D8" t="s" s="0">
         <v>34</v>
@@ -550,7 +553,7 @@
         <v>34</v>
       </c>
       <c r="F8" t="s" s="0">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="G8" t="n" s="0">
         <v>1000000.0</v>
@@ -568,7 +571,7 @@
         <v>17</v>
       </c>
       <c r="L8" t="s" s="0">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9">
@@ -576,10 +579,10 @@
         <v>9.0</v>
       </c>
       <c r="B9" t="s" s="0">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s" s="0">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D9" t="s" s="0">
         <v>27</v>
@@ -588,7 +591,7 @@
         <v>33</v>
       </c>
       <c r="F9" t="s" s="0">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G9" t="n" s="0">
         <v>1000000.0</v>
@@ -603,10 +606,10 @@
         <v>1.0</v>
       </c>
       <c r="K9" t="s" s="0">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="L9" t="s" s="0">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10">
@@ -614,10 +617,10 @@
         <v>10.0</v>
       </c>
       <c r="B10" t="s" s="0">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C10" t="s" s="0">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D10" t="s" s="0">
         <v>34</v>
@@ -626,16 +629,16 @@
         <v>33</v>
       </c>
       <c r="F10" t="s" s="0">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="G10" t="n" s="0">
         <v>1000000.0</v>
       </c>
       <c r="H10" t="n" s="0">
-        <v>45343.0</v>
+        <v>45358.0</v>
       </c>
       <c r="I10" t="n" s="0">
-        <v>45343.0</v>
+        <v>45358.0</v>
       </c>
       <c r="J10" t="n" s="0">
         <v>1.0</v>
@@ -644,7 +647,7 @@
         <v>29</v>
       </c>
       <c r="L10" t="s" s="0">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11">
@@ -652,10 +655,10 @@
         <v>11.0</v>
       </c>
       <c r="B11" t="s" s="0">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C11" t="s" s="0">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="D11" t="s" s="0">
         <v>33</v>
@@ -664,7 +667,7 @@
         <v>33</v>
       </c>
       <c r="F11" t="s" s="0">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="G11" t="n" s="0">
         <v>1000000.0</v>
@@ -679,10 +682,10 @@
         <v>1.0</v>
       </c>
       <c r="K11" t="s" s="0">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="L11" t="s" s="0">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
   </sheetData>

</xml_diff>